<commit_message>
feat(abc:xlsx): add xlsx component
</commit_message>
<xml_diff>
--- a/src/assets/demo.xlsx
+++ b/src/assets/demo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asdf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asdf\Desktop\work\delon\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -54,8 +54,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -370,12 +371,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+      <c r="C2" s="1">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>